<commit_message>
Teminados todos los puntos importantes de la documentacion
</commit_message>
<xml_diff>
--- a/doc/anexos/Capítulo 11. Presupuesto final.xlsx
+++ b/doc/anexos/Capítulo 11. Presupuesto final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xamel\Dropbox\Uniovi\TFG\ElFavorDeLasGuerreras\doc\anexos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5946BC-FB4F-46C4-8936-50EBCD77F9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A561BF16-AF8B-46A0-8279-16756B2277A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificacion_Final" sheetId="2" r:id="rId1"/>
@@ -1098,7 +1098,7 @@
                   <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>73</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2230,7 +2230,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8AA03D-9082-4234-9404-AB9320BC371F}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2266,7 +2268,7 @@
       </c>
       <c r="D2" s="67">
         <f>SUM(D3:D7)</f>
-        <v>432</v>
+        <v>441</v>
       </c>
       <c r="E2" s="68"/>
     </row>
@@ -2353,7 +2355,7 @@
         <v>40</v>
       </c>
       <c r="D7" s="71">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E7" s="76" t="str">
         <f>'Coste de personal'!A3</f>
@@ -2749,7 +2751,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E86D725C-4884-4A2C-9459-00B6F79789CA}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N6" sqref="L3:N6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2812,7 +2816,7 @@
       </c>
       <c r="B3" s="35">
         <f>Planificacion_Final!D2</f>
-        <v>432</v>
+        <v>441</v>
       </c>
       <c r="C3" s="35" t="s">
         <v>31</v>
@@ -2821,14 +2825,14 @@
       <c r="E3" s="41"/>
       <c r="F3" s="42">
         <f>SUM(F4:F8)</f>
-        <v>9437.98</v>
+        <v>9650.65</v>
       </c>
       <c r="H3" s="30">
         <v>6122.2999999999984</v>
       </c>
       <c r="I3" s="30">
         <f>Tabla7[[#This Row],[Total]]</f>
-        <v>9437.98</v>
+        <v>9650.65</v>
       </c>
       <c r="J3"/>
       <c r="K3" s="62" t="s">
@@ -2839,11 +2843,11 @@
       </c>
       <c r="M3" s="63">
         <f>I3</f>
-        <v>9437.98</v>
+        <v>9650.65</v>
       </c>
       <c r="N3" s="57">
         <f>M3-L3</f>
-        <v>3315.6800000000012</v>
+        <v>3528.3500000000013</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2879,11 +2883,11 @@
       </c>
       <c r="M4" s="63">
         <f>(M3*I9)</f>
-        <v>2359.4949999999999</v>
+        <v>2412.6624999999999</v>
       </c>
       <c r="N4" s="57">
         <f t="shared" ref="N4:N6" si="0">M4-L4</f>
-        <v>828.9200000000003</v>
+        <v>882.08750000000032</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -2971,11 +2975,11 @@
       </c>
       <c r="M6" s="60">
         <f>SUM(M3:M5)</f>
-        <v>13717.474999999999</v>
+        <v>13983.3125</v>
       </c>
       <c r="N6" s="61">
         <f t="shared" si="0"/>
-        <v>5584.6</v>
+        <v>5850.4375000000018</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3013,7 +3017,7 @@
       </c>
       <c r="B8" s="38">
         <f>Planificacion_Final!D7</f>
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="C8" s="38" t="s">
         <v>31</v>
@@ -3028,7 +3032,7 @@
       </c>
       <c r="F8" s="41">
         <f>(Tabla7[[#This Row],[Coste por hora]]*Tabla7[[#This Row],[Cantidad]])</f>
-        <v>1724.99</v>
+        <v>1937.6599999999999</v>
       </c>
       <c r="H8" s="21" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Corrección de errores y cambios en la documentacion
</commit_message>
<xml_diff>
--- a/doc/anexos/Capítulo 11. Presupuesto final.xlsx
+++ b/doc/anexos/Capítulo 11. Presupuesto final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xamel\Dropbox\Uniovi\TFG\ElFavorDeLasGuerreras\doc\anexos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Uniovi\TFG\ElFavorDeLasGuerreras\doc\anexos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A561BF16-AF8B-46A0-8279-16756B2277A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643DCC85-8F15-4B35-88BD-82B59471C9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificacion_Final" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t>Nombre de la tarea</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>Beneficio esperado del 25%</t>
+  </si>
+  <si>
+    <t>Alquiler de software</t>
+  </si>
+  <si>
+    <t>Gastos de reparación de hardware</t>
   </si>
 </sst>
 </file>
@@ -1092,13 +1098,13 @@
                   <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>82</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2230,9 +2236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8AA03D-9082-4234-9404-AB9320BC371F}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2268,7 +2272,7 @@
       </c>
       <c r="D2" s="67">
         <f>SUM(D3:D7)</f>
-        <v>441</v>
+        <v>456</v>
       </c>
       <c r="E2" s="68"/>
     </row>
@@ -2319,7 +2323,7 @@
         <v>85</v>
       </c>
       <c r="D5" s="71">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="E5" s="76" t="str">
         <f>'Coste de personal'!A4</f>
@@ -2355,7 +2359,7 @@
         <v>40</v>
       </c>
       <c r="D7" s="71">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="E7" s="76" t="str">
         <f>'Coste de personal'!A3</f>
@@ -2625,9 +2629,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9CE8C43-6D0A-4601-A1B0-A769CFC83B6E}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="A2:D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2656,7 +2662,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="45">
-        <f>B13</f>
+        <f>B15</f>
         <v>16</v>
       </c>
       <c r="C2" s="19">
@@ -2672,7 +2678,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="45">
-        <f>B13</f>
+        <f>B15</f>
         <v>16</v>
       </c>
       <c r="C3" s="19">
@@ -2685,60 +2691,92 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B4" s="45">
-        <f>B13</f>
+        <f>B15</f>
         <v>16</v>
       </c>
       <c r="C4" s="19">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D4" s="19">
         <f>C4*B4</f>
-        <v>320</v>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="45">
+        <f>B15</f>
+        <v>16</v>
+      </c>
+      <c r="C5" s="19">
+        <v>40</v>
+      </c>
+      <c r="D5" s="19">
+        <f t="shared" ref="D5:D6" si="0">C5*B5</f>
+        <v>640</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="45">
+        <f>B15</f>
+        <v>16</v>
+      </c>
+      <c r="C6" s="19">
+        <v>150</v>
+      </c>
+      <c r="D6" s="19">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="20">
-        <f>SUM(D2:D4)</f>
-        <v>1920</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="47">
-        <v>44228</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="47">
-        <v>44713</v>
+      <c r="B8" s="20">
+        <f>SUM(D2:D6)</f>
+        <v>5280</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="48">
-        <f>(B11-B10)*(12/365)</f>
-        <v>15.945205479452053</v>
+        <v>41</v>
+      </c>
+      <c r="B12" s="47">
+        <v>44228</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="47">
+        <v>44713</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="48">
+        <f>(B13-B12)*(12/365)</f>
+        <v>15.945205479452053</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="49">
-        <f>ROUND(B12, 0)</f>
+      <c r="B15" s="49">
+        <f>ROUND(B14, 0)</f>
         <v>16</v>
       </c>
     </row>
@@ -2751,7 +2789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E86D725C-4884-4A2C-9459-00B6F79789CA}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N6" sqref="L3:N6"/>
     </sheetView>
   </sheetViews>
@@ -2816,7 +2854,7 @@
       </c>
       <c r="B3" s="35">
         <f>Planificacion_Final!D2</f>
-        <v>441</v>
+        <v>456</v>
       </c>
       <c r="C3" s="35" t="s">
         <v>31</v>
@@ -2825,14 +2863,14 @@
       <c r="E3" s="41"/>
       <c r="F3" s="42">
         <f>SUM(F4:F8)</f>
-        <v>9650.65</v>
+        <v>9943.06</v>
       </c>
       <c r="H3" s="30">
         <v>6122.2999999999984</v>
       </c>
       <c r="I3" s="30">
         <f>Tabla7[[#This Row],[Total]]</f>
-        <v>9650.65</v>
+        <v>9943.06</v>
       </c>
       <c r="J3"/>
       <c r="K3" s="62" t="s">
@@ -2843,11 +2881,11 @@
       </c>
       <c r="M3" s="63">
         <f>I3</f>
-        <v>9650.65</v>
+        <v>9943.06</v>
       </c>
       <c r="N3" s="57">
         <f>M3-L3</f>
-        <v>3528.3500000000013</v>
+        <v>3820.7600000000011</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2883,11 +2921,11 @@
       </c>
       <c r="M4" s="63">
         <f>(M3*I9)</f>
-        <v>2412.6624999999999</v>
+        <v>2485.7649999999999</v>
       </c>
       <c r="N4" s="57">
         <f t="shared" ref="N4:N6" si="0">M4-L4</f>
-        <v>882.08750000000032</v>
+        <v>955.19000000000028</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -2929,11 +2967,11 @@
       </c>
       <c r="M5" s="63">
         <f>I12</f>
-        <v>1920</v>
+        <v>5280</v>
       </c>
       <c r="N5" s="57">
         <f t="shared" si="0"/>
-        <v>1440</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2943,7 +2981,7 @@
       </c>
       <c r="B6" s="38">
         <f>Planificacion_Final!D5</f>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C6" s="38" t="s">
         <v>31</v>
@@ -2958,7 +2996,7 @@
       </c>
       <c r="F6" s="41">
         <f>(Tabla7[[#This Row],[Coste por hora]]*Tabla7[[#This Row],[Cantidad]])</f>
-        <v>1329</v>
+        <v>1408.74</v>
       </c>
       <c r="H6" s="29">
         <v>0</v>
@@ -2975,11 +3013,11 @@
       </c>
       <c r="M6" s="60">
         <f>SUM(M3:M5)</f>
-        <v>13983.3125</v>
+        <v>17708.824999999997</v>
       </c>
       <c r="N6" s="61">
         <f t="shared" si="0"/>
-        <v>5850.4375000000018</v>
+        <v>9575.9499999999989</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3017,7 +3055,7 @@
       </c>
       <c r="B8" s="38">
         <f>Planificacion_Final!D7</f>
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C8" s="38" t="s">
         <v>31</v>
@@ -3032,7 +3070,7 @@
       </c>
       <c r="F8" s="41">
         <f>(Tabla7[[#This Row],[Coste por hora]]*Tabla7[[#This Row],[Cantidad]])</f>
-        <v>1937.6599999999999</v>
+        <v>2150.33</v>
       </c>
       <c r="H8" s="21" t="s">
         <v>24</v>
@@ -3070,8 +3108,8 @@
         <v>480</v>
       </c>
       <c r="I12" s="23">
-        <f>'Costes indirectos'!B6</f>
-        <v>1920</v>
+        <f>'Costes indirectos'!B8</f>
+        <v>5280</v>
       </c>
       <c r="J12"/>
     </row>

</xml_diff>